<commit_message>
MeF du Excel TI ok, Impact_poste avec min et max
</commit_message>
<xml_diff>
--- a/Excel/TI/Mon_TI_2024_02_15.xlsx
+++ b/Excel/TI/Mon_TI_2024_02_15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK10"/>
+  <dimension ref="A1:AK9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -623,58 +623,58 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Giannis Antetokounmpo</t>
+          <t>Anthony Edwards</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="D2" t="inlineStr"/>
       <c r="E2" t="n">
-        <v>49.6</v>
+        <v>45.4</v>
       </c>
       <c r="F2" t="n">
-        <v>51.5</v>
+        <v>36.7</v>
       </c>
       <c r="G2" t="n">
-        <v>53.9</v>
+        <v>36.6</v>
       </c>
       <c r="H2" t="n">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L2" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="M2" t="n">
+        <v>58</v>
+      </c>
+      <c r="N2" t="n">
+        <v>33</v>
+      </c>
+      <c r="O2" t="n">
         <v>36</v>
       </c>
-      <c r="N2" t="n">
-        <v>22</v>
-      </c>
-      <c r="O2" t="n">
-        <v>47</v>
-      </c>
       <c r="P2" t="n">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q2" t="n">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="R2" t="inlineStr">
         <is>
@@ -683,84 +683,82 @@
       </c>
       <c r="S2" t="inlineStr">
         <is>
+          <t>POR</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="U2" t="n">
+        <v>58</v>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="W2" t="n">
+        <v>16</v>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>MIL</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>SAS</t>
+        </is>
+      </c>
+      <c r="AF2" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AG2" t="inlineStr">
+        <is>
           <t>MEM</t>
         </is>
       </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="U2" t="n">
-        <v>50</v>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>MIN</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="AF2" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AG2" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
       <c r="AH2" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI2" t="n">
-        <v>-2.8</v>
+        <v>-1</v>
       </c>
       <c r="AJ2" t="inlineStr"/>
       <c r="AK2" t="inlineStr"/>
@@ -783,19 +781,19 @@
       </c>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="n">
-        <v>42.8</v>
+        <v>36.6</v>
       </c>
       <c r="F3" t="n">
-        <v>31.5</v>
+        <v>29.7</v>
       </c>
       <c r="G3" t="n">
-        <v>29.4</v>
+        <v>28.8</v>
       </c>
       <c r="H3" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" t="n">
         <v>2</v>
@@ -807,23 +805,23 @@
         <v>4</v>
       </c>
       <c r="M3" t="n">
+        <v>5</v>
+      </c>
+      <c r="N3" t="n">
         <v>29</v>
       </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
         <v>74</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="P3" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="Q3" t="n">
-        <v>30</v>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="R3" t="inlineStr">
         <is>
@@ -837,22 +835,20 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="U3" t="n">
+        <v>5</v>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="W3" t="n">
         <v>9</v>
       </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
       <c r="X3" t="inlineStr">
         <is>
           <t>-</t>
@@ -909,7 +905,7 @@
         </is>
       </c>
       <c r="AI3" t="n">
-        <v>5</v>
+        <v>4.3</v>
       </c>
       <c r="AJ3" t="inlineStr"/>
       <c r="AK3" t="inlineStr"/>
@@ -917,67 +913,71 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Anthony Edwards</t>
+          <t>Lauri Markkanen</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>F-C</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
       <c r="E4" t="n">
-        <v>35.8</v>
+        <v>30.6</v>
       </c>
       <c r="F4" t="n">
-        <v>35.6</v>
+        <v>35.5</v>
       </c>
       <c r="G4" t="n">
-        <v>36.2</v>
+        <v>35.9</v>
       </c>
       <c r="H4" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K4" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L4" t="n">
         <v>5</v>
       </c>
       <c r="M4" t="n">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="N4" t="n">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="O4" t="n">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="P4" t="n">
-        <v>23</v>
+        <v>58</v>
       </c>
       <c r="Q4" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="R4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="S4" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="T4" t="inlineStr">
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="U4" t="n">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="V4" t="inlineStr">
         <is>
@@ -1015,7 +1015,7 @@
       </c>
       <c r="AA4" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AB4" t="inlineStr">
@@ -1025,129 +1025,125 @@
       </c>
       <c r="AC4" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>SAS</t>
         </is>
       </c>
       <c r="AD4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AE4" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>ATL</t>
         </is>
       </c>
       <c r="AF4" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AG4" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>ORL</t>
         </is>
       </c>
       <c r="AH4" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AI4" t="n">
-        <v>-1.4</v>
-      </c>
-      <c r="AJ4" t="inlineStr"/>
-      <c r="AK4" t="inlineStr"/>
+        <v>2.3</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>-0.5</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>UTA</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lauri Markkanen</t>
+          <t>Karl-Anthony Towns</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>F-C</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
+          <t>C-F</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="n">
-        <v>35.2</v>
+        <v>30.2</v>
       </c>
       <c r="F5" t="n">
-        <v>38.7</v>
+        <v>36.3</v>
       </c>
       <c r="G5" t="n">
-        <v>36.6</v>
+        <v>35.7</v>
       </c>
       <c r="H5" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>5</v>
+      </c>
+      <c r="K5" t="n">
         <v>3</v>
-      </c>
-      <c r="J5" t="n">
-        <v>3</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0</v>
       </c>
       <c r="L5" t="n">
         <v>6</v>
       </c>
       <c r="M5" t="n">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="N5" t="n">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="O5" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P5" t="n">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="Q5" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="R5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="S5" t="inlineStr">
         <is>
-          <t>GSW</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="T5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="U5" t="n">
+        <v>21</v>
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W5" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="W5" t="n">
+        <v>48</v>
       </c>
       <c r="X5" t="inlineStr">
         <is>
@@ -1166,7 +1162,7 @@
       </c>
       <c r="AA5" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="AB5" t="inlineStr">
@@ -1176,99 +1172,99 @@
       </c>
       <c r="AC5" t="inlineStr">
         <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="AD5" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AE5" t="inlineStr">
+        <is>
           <t>SAS</t>
         </is>
       </c>
-      <c r="AD5" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AE5" t="inlineStr">
-        <is>
-          <t>ATL</t>
-        </is>
-      </c>
       <c r="AF5" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AG5" t="inlineStr">
         <is>
-          <t>ORL</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="AH5" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI5" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>-1.3</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>6</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>MIL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Karl-Anthony Towns</t>
+          <t>Damian Lillard</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>C-F</t>
+          <t>G</t>
         </is>
       </c>
       <c r="D6" t="inlineStr"/>
       <c r="E6" t="n">
-        <v>31.6</v>
+        <v>28.4</v>
       </c>
       <c r="F6" t="n">
-        <v>37.3</v>
+        <v>32.8</v>
       </c>
       <c r="G6" t="n">
-        <v>35.9</v>
+        <v>35.4</v>
       </c>
       <c r="H6" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I6" t="n">
+        <v>4</v>
+      </c>
+      <c r="J6" t="n">
+        <v>4</v>
+      </c>
+      <c r="K6" t="n">
         <v>1</v>
       </c>
-      <c r="J6" t="n">
-        <v>5</v>
-      </c>
-      <c r="K6" t="n">
-        <v>2</v>
-      </c>
       <c r="L6" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="M6" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="N6" t="n">
+        <v>24</v>
+      </c>
+      <c r="O6" t="n">
         <v>43</v>
       </c>
-      <c r="O6" t="n">
-        <v>24</v>
-      </c>
-      <c r="P6" t="n">
-        <v>16</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>50</v>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="R6" t="inlineStr">
         <is>
@@ -1277,16 +1273,18 @@
       </c>
       <c r="S6" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>MEM</t>
         </is>
       </c>
       <c r="T6" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="U6" t="n">
-        <v>26</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="V6" t="inlineStr">
         <is>
@@ -1310,22 +1308,22 @@
       </c>
       <c r="Z6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AA6" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>MIN</t>
         </is>
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>PHI</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr">
@@ -1335,17 +1333,17 @@
       </c>
       <c r="AE6" t="inlineStr">
         <is>
-          <t>SAS</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AF6" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AG6" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AH6" t="inlineStr">
@@ -1354,7 +1352,7 @@
         </is>
       </c>
       <c r="AI6" t="n">
-        <v>1.8</v>
+        <v>-1</v>
       </c>
       <c r="AJ6" t="inlineStr"/>
       <c r="AK6" t="inlineStr"/>
@@ -1362,80 +1360,84 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>MEM</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Jaren Jackson Jr.</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>F-C</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+      <c r="E7" t="n">
+        <v>28.4</v>
+      </c>
+      <c r="F7" t="n">
+        <v>29.1</v>
+      </c>
+      <c r="G7" t="n">
+        <v>30.2</v>
+      </c>
+      <c r="H7" t="n">
+        <v>13</v>
+      </c>
+      <c r="I7" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" t="n">
+        <v>7</v>
+      </c>
+      <c r="L7" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" t="n">
+        <v>22</v>
+      </c>
+      <c r="N7" t="n">
+        <v>24</v>
+      </c>
+      <c r="O7" t="n">
+        <v>35</v>
+      </c>
+      <c r="P7" t="n">
+        <v>28</v>
+      </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
           <t>MIL</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Damian Lillard</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>G</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>30.8</v>
-      </c>
-      <c r="F7" t="n">
-        <v>33.7</v>
-      </c>
-      <c r="G7" t="n">
-        <v>36.1</v>
-      </c>
-      <c r="H7" t="n">
-        <v>12</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" t="n">
-        <v>3</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" t="n">
-        <v>4</v>
-      </c>
-      <c r="M7" t="n">
-        <v>43</v>
-      </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P7" t="n">
-        <v>4</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>54</v>
-      </c>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>MEM</t>
-        </is>
-      </c>
       <c r="T7" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="U7" t="n">
-        <v>26</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="V7" t="inlineStr">
         <is>
@@ -1459,42 +1461,42 @@
       </c>
       <c r="Z7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AA7" t="inlineStr">
         <is>
+          <t>LAC</t>
+        </is>
+      </c>
+      <c r="AB7" t="inlineStr">
+        <is>
+          <t>vs</t>
+        </is>
+      </c>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>BKN</t>
+        </is>
+      </c>
+      <c r="AD7" t="inlineStr">
+        <is>
+          <t>@</t>
+        </is>
+      </c>
+      <c r="AE7" t="inlineStr">
+        <is>
           <t>MIN</t>
         </is>
       </c>
-      <c r="AB7" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AC7" t="inlineStr">
-        <is>
-          <t>PHI</t>
-        </is>
-      </c>
-      <c r="AD7" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AE7" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
       <c r="AF7" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AG7" t="inlineStr">
         <is>
-          <t>CHA</t>
+          <t>POR</t>
         </is>
       </c>
       <c r="AH7" t="inlineStr">
@@ -1503,25 +1505,29 @@
         </is>
       </c>
       <c r="AI7" t="n">
-        <v>1.4</v>
-      </c>
-      <c r="AJ7" t="inlineStr"/>
-      <c r="AK7" t="inlineStr"/>
+        <v>-2.2</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MEM</t>
+          <t>GSW</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jaren Jackson Jr.</t>
+          <t>Andrew Wiggins</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>F-C</t>
+          <t>F</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1530,56 +1536,52 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>29.8</v>
+        <v>24</v>
       </c>
       <c r="F8" t="n">
-        <v>32.8</v>
+        <v>22</v>
       </c>
       <c r="G8" t="n">
-        <v>30.5</v>
+        <v>17</v>
       </c>
       <c r="H8" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="J8" t="n">
         <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="N8" t="n">
-        <v>28</v>
-      </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
+        <v>25</v>
+      </c>
+      <c r="O8" t="n">
+        <v>17</v>
+      </c>
+      <c r="P8" t="n">
+        <v>20</v>
       </c>
       <c r="Q8" t="n">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t>MIL</t>
+          <t>UTA</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1588,23 +1590,27 @@
         </is>
       </c>
       <c r="U8" t="n">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="V8" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="W8" t="n">
-        <v>39</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="W8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="X8" t="inlineStr">
         <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="Y8" t="n">
-        <v>12</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="Z8" t="inlineStr">
         <is>
@@ -1613,7 +1619,7 @@
       </c>
       <c r="AA8" t="inlineStr">
         <is>
-          <t>LAC</t>
+          <t>LAL</t>
         </is>
       </c>
       <c r="AB8" t="inlineStr">
@@ -1623,42 +1629,42 @@
       </c>
       <c r="AC8" t="inlineStr">
         <is>
-          <t>BKN</t>
+          <t>CHA</t>
         </is>
       </c>
       <c r="AD8" t="inlineStr">
         <is>
-          <t>@</t>
+          <t>vs</t>
         </is>
       </c>
       <c r="AE8" t="inlineStr">
         <is>
-          <t>MIN</t>
+          <t>DEN</t>
         </is>
       </c>
       <c r="AF8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AG8" t="inlineStr">
         <is>
-          <t>POR</t>
+          <t>WAS</t>
         </is>
       </c>
       <c r="AH8" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI8" t="n">
-        <v>-2.1</v>
+        <v>0.8</v>
       </c>
       <c r="AJ8" t="n">
-        <v>4.2</v>
+        <v>-4.5</v>
       </c>
       <c r="AK8" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9">
@@ -1712,17 +1718,19 @@
           <t>-</t>
         </is>
       </c>
-      <c r="O9" t="n">
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
         <v>12</v>
       </c>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q9" t="n">
-        <v>18</v>
-      </c>
       <c r="R9" t="inlineStr">
         <is>
           <t>@</t>
@@ -1735,11 +1743,13 @@
       </c>
       <c r="T9" t="inlineStr">
         <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="U9" t="n">
-        <v>22</v>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="U9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
       </c>
       <c r="V9" t="inlineStr">
         <is>
@@ -1803,171 +1813,14 @@
       </c>
       <c r="AH9" t="inlineStr">
         <is>
-          <t>vs</t>
+          <t>@</t>
         </is>
       </c>
       <c r="AI9" t="n">
-        <v>1</v>
+        <v>-0.8</v>
       </c>
       <c r="AJ9" t="inlineStr"/>
       <c r="AK9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>GSW</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Andrew Wiggins</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>F</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>O</t>
-        </is>
-      </c>
-      <c r="E10" t="n">
-        <v>18.4</v>
-      </c>
-      <c r="F10" t="n">
-        <v>19.2</v>
-      </c>
-      <c r="G10" t="n">
-        <v>16.8</v>
-      </c>
-      <c r="H10" t="n">
-        <v>10</v>
-      </c>
-      <c r="I10" t="n">
-        <v>4</v>
-      </c>
-      <c r="J10" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" t="n">
-        <v>3</v>
-      </c>
-      <c r="L10" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" t="n">
-        <v>17</v>
-      </c>
-      <c r="N10" t="n">
-        <v>20</v>
-      </c>
-      <c r="O10" t="n">
-        <v>39</v>
-      </c>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Q10" t="n">
-        <v>2</v>
-      </c>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>UTA</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="V10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="W10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>LAL</t>
-        </is>
-      </c>
-      <c r="AB10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AC10" t="inlineStr">
-        <is>
-          <t>CHA</t>
-        </is>
-      </c>
-      <c r="AD10" t="inlineStr">
-        <is>
-          <t>vs</t>
-        </is>
-      </c>
-      <c r="AE10" t="inlineStr">
-        <is>
-          <t>DEN</t>
-        </is>
-      </c>
-      <c r="AF10" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AG10" t="inlineStr">
-        <is>
-          <t>WAS</t>
-        </is>
-      </c>
-      <c r="AH10" t="inlineStr">
-        <is>
-          <t>@</t>
-        </is>
-      </c>
-      <c r="AI10" t="n">
-        <v>0.7</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>-4.2</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>